<commit_message>
chrome update to mozilla
</commit_message>
<xml_diff>
--- a/Bug Tracker _ Amnet Digital 2.0.xlsx
+++ b/Bug Tracker _ Amnet Digital 2.0.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dayan\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dayan\Desktop\QA files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74C94F51-0350-4960-AA60-50B76590BEBB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F2FC3EA-6EA4-4980-B26E-542196578622}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{594BC756-E5B0-4631-A474-73C52B5FE5F2}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="69">
   <si>
     <t>Screen Name</t>
   </si>
@@ -230,6 +230,9 @@
   </si>
   <si>
     <t xml:space="preserve">Contact Us Backgroud clolor not as per design </t>
+  </si>
+  <si>
+    <t>Mozilla</t>
   </si>
 </sst>
 </file>
@@ -615,7 +618,7 @@
   <dimension ref="A1:D62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -678,7 +681,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
-        <v>5</v>
+        <v>68</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>

</xml_diff>